<commit_message>
first attempt for micortsoft calendar
</commit_message>
<xml_diff>
--- a/events1.xlsx
+++ b/events1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://apworkspace-my.sharepoint.com/personal/ivan_cheung_arrowpointfund_com/Documents/Documents/arrowpoint/winter/calendar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{619B5A14-3B94-4244-9526-C9EACE5E3229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{619B5A14-3B94-4244-9526-C9EACE5E3229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D47CE13E-D4D6-4D09-8830-52CAC86EE6A1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4359,8 +4359,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="#,##0.00##_);[Red]\(#,##0.00##\)"/>
-    <numFmt numFmtId="179" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00##_);[Red]\(#,##0.00##\)"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -4847,7 +4847,7 @@
     <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -4867,15 +4867,15 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" xfId="27"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="26"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="26"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="28"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="45"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="46"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="46"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -5228,7 +5228,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF843"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5248,7 +5250,8 @@
     <col min="15" max="15" width="10.42578125" customWidth="1"/>
     <col min="16" max="16" width="9.5703125" customWidth="1"/>
     <col min="17" max="17" width="14.28515625" customWidth="1"/>
-    <col min="18" max="21" width="9.5703125" customWidth="1"/>
+    <col min="18" max="20" width="9.5703125" customWidth="1"/>
+    <col min="21" max="21" width="19.85546875" customWidth="1"/>
     <col min="22" max="22" width="14.28515625" customWidth="1"/>
     <col min="23" max="23" width="15.28515625" customWidth="1"/>
     <col min="24" max="24" width="4.7109375" customWidth="1"/>
@@ -5368,7 +5371,7 @@
         <v>33</v>
       </c>
       <c r="C2" s="4">
-        <v>46027.791666666701</v>
+        <v>46027.791666666664</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>34</v>

</xml_diff>